<commit_message>
Add another project and photos
</commit_message>
<xml_diff>
--- a/المشاريع مصنفة.xlsx
+++ b/المشاريع مصنفة.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\عاصم ملفات\الجمعية\2025\المشاريع والأنشطة\RePort2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0076DD73-E3D8-4E53-A723-63334C4C9064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB0132B-51D3-4DE8-92C1-D82CBE2EDD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="الاستجابة" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="اعادة الروابط" sheetId="5" r:id="rId4"/>
     <sheet name="التوعية بمخاطر الألغام  " sheetId="6" r:id="rId5"/>
     <sheet name=" (نقل سيارات الاسعاف)الإحالة" sheetId="7" r:id="rId6"/>
+    <sheet name="الإعلام التعريف بالحركة الدولية" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">التدريب!$A$1:$J$1</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="185">
   <si>
     <t>رقم المشروع</t>
   </si>
@@ -406,15 +407,6 @@
   </si>
   <si>
     <t xml:space="preserve">الإجمالي </t>
-  </si>
-  <si>
-    <t>تعريف بأنشطة الجمعية (نساء)</t>
-  </si>
-  <si>
-    <t>تعريف بأنشطة الجمعية (رجال)</t>
-  </si>
-  <si>
-    <t>تعريف بأنشطة الجمعية (أطفال)</t>
   </si>
   <si>
     <t>مشاركة لخط الساخن</t>
@@ -537,13 +529,85 @@
   </si>
   <si>
     <t>أبريل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الربع </t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدد المستفيدين </t>
+  </si>
+  <si>
+    <t>المديرية / المنطقة</t>
+  </si>
+  <si>
+    <t>المستهدفين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الأول </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ورشة </t>
+  </si>
+  <si>
+    <t>المدينة - مبنى الفرع</t>
+  </si>
+  <si>
+    <t>وجهاء المجتمع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جلسة </t>
+  </si>
+  <si>
+    <t>حريب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">المجتمع </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الثاني </t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعلاميين </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الرويك </t>
+  </si>
+  <si>
+    <t>الثالث</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مكاتب حكومية </t>
+  </si>
+  <si>
+    <t xml:space="preserve">حريب </t>
+  </si>
+  <si>
+    <t xml:space="preserve">مجتمع محلي </t>
+  </si>
+  <si>
+    <t>الرابع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عقال حارات </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الوادي / الرويك </t>
+  </si>
+  <si>
+    <t xml:space="preserve">كجتمع محلي </t>
+  </si>
+  <si>
+    <t>تعريف بأنشطة الجمعية</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,24 +620,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="178"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="178"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="178"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -634,6 +699,7 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -672,6 +738,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -685,27 +752,32 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -714,8 +786,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,8 +914,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -993,6 +1085,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1002,7 +1107,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1176,6 +1281,27 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="13" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="13" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="عادي" xfId="0" builtinId="0"/>
@@ -1205,8 +1331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F8E8E9F-9143-44F5-93B9-95F1CD1BD7A7}" name="الجدول1" displayName="الجدول1" ref="A17:D20" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="A17:D20" xr:uid="{9CBFF556-F4B4-467B-B6A6-CA252F602F85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F8E8E9F-9143-44F5-93B9-95F1CD1BD7A7}" name="الجدول1" displayName="الجدول1" ref="A15:D18" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A15:D18" xr:uid="{9CBFF556-F4B4-467B-B6A6-CA252F602F85}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F666BA90-44E0-48E0-8EAA-04FD2A6C32B9}" name="النشاط"/>
     <tableColumn id="2" xr3:uid="{43609D6E-6FAC-40DE-AF3B-12CAD30D6AB8}" name="العدد رجال"/>
@@ -1524,7 +1650,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.69921875" bestFit="1" customWidth="1"/>
@@ -1537,7 +1663,7 @@
     <col min="10" max="10" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1601,7 +1727,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1633,7 +1759,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1665,7 +1791,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1697,7 +1823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1729,7 +1855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1761,7 +1887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1793,7 +1919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1825,7 +1951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1857,7 +1983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="41.4">
+    <row r="11" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1889,7 +2015,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1921,7 +2047,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1953,7 +2079,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1985,7 +2111,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2014,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2046,7 +2172,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2078,7 +2204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2110,7 +2236,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2142,7 +2268,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2174,7 +2300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2206,7 +2332,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
         <v>98</v>
       </c>
@@ -2239,7 +2365,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.296875" bestFit="1" customWidth="1"/>
@@ -2253,7 +2379,7 @@
     <col min="10" max="10" width="13.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -2285,7 +2411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2317,7 +2443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="27.6">
+    <row r="3" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2349,7 +2475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2381,7 +2507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.6">
+    <row r="5" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2413,7 +2539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2443,7 +2569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
         <v>99</v>
       </c>
@@ -2481,7 +2607,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="42.8984375" customWidth="1"/>
@@ -2494,7 +2620,7 @@
     <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
@@ -2526,7 +2652,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2558,7 +2684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2590,7 +2716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2619,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2651,7 +2777,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2683,7 +2809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>103</v>
       </c>
@@ -2715,13 +2841,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E207662D-8C05-4F1B-8596-025837BE8D63}">
-  <dimension ref="A4:N20"/>
+  <dimension ref="A4:N18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.59765625" style="14" customWidth="1"/>
     <col min="2" max="2" width="17.09765625" style="14" customWidth="1"/>
@@ -2729,12 +2855,12 @@
     <col min="4" max="16384" width="8.796875" style="14"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:14" ht="21.6">
+    <row r="4" spans="1:14" ht="21.6" x14ac:dyDescent="0.7">
       <c r="C4" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17.399999999999999">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>107</v>
       </c>
@@ -2778,366 +2904,276 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.6">
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="B7" s="19">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="C7" s="20">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D7" s="21">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E7" s="21">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="F7" s="21">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="G7" s="21">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="H7" s="21">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="I7" s="22">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="J7" s="22">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="K7" s="22">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="L7" s="22">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="M7" s="22">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="N7" s="17">
         <f>SUM(B7:M7)</f>
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.6">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="19">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="C8" s="20">
-        <v>58</v>
-      </c>
-      <c r="D8" s="20">
-        <v>34</v>
-      </c>
-      <c r="E8" s="20">
-        <v>51</v>
-      </c>
-      <c r="F8" s="20">
-        <v>41</v>
-      </c>
-      <c r="G8" s="20">
-        <v>39</v>
-      </c>
-      <c r="H8" s="20">
-        <v>80</v>
-      </c>
-      <c r="I8" s="22">
-        <v>76</v>
-      </c>
-      <c r="J8" s="22">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="21">
+        <v>15</v>
+      </c>
+      <c r="E8" s="21">
+        <v>15</v>
+      </c>
+      <c r="F8" s="21">
+        <v>11</v>
+      </c>
+      <c r="G8" s="21">
+        <v>10</v>
+      </c>
+      <c r="H8" s="21">
+        <v>11</v>
+      </c>
+      <c r="I8" s="23">
+        <v>12</v>
+      </c>
+      <c r="J8" s="23">
+        <v>14</v>
       </c>
       <c r="K8" s="22">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="L8" s="22">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="M8" s="22">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="N8" s="17">
         <f>SUM(B8:M8)</f>
-        <v>696</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.6">
-      <c r="A9" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="19">
+        <f>SUM(B7:B8)</f>
+        <v>124</v>
+      </c>
+      <c r="C9" s="19">
+        <f>SUM(C7:C8)</f>
+        <v>121</v>
+      </c>
+      <c r="D9" s="19">
+        <f>SUM(D7:D8)</f>
+        <v>88</v>
+      </c>
+      <c r="E9" s="19">
+        <f>SUM(E7:E8)</f>
+        <v>108</v>
+      </c>
+      <c r="F9" s="19">
+        <f>SUM(F7:F8)</f>
+        <v>102</v>
+      </c>
+      <c r="G9" s="19">
+        <f>SUM(G7:G8)</f>
+        <v>76</v>
+      </c>
+      <c r="H9" s="19">
+        <f>SUM(H7:H8)</f>
+        <v>124</v>
+      </c>
+      <c r="I9" s="19">
+        <f>SUM(I7:I8)</f>
+        <v>127</v>
+      </c>
+      <c r="J9" s="19">
+        <f>SUM(J7:J8)</f>
+        <v>137</v>
+      </c>
+      <c r="K9" s="19">
+        <f>SUM(K7:K8)</f>
+        <v>91</v>
+      </c>
+      <c r="L9" s="19">
+        <f>SUM(L7:L8)</f>
+        <v>87</v>
+      </c>
+      <c r="M9" s="19">
+        <f>SUM(M7:M8)</f>
+        <v>116</v>
+      </c>
+      <c r="N9" s="25">
+        <f>SUM(N7:N8)</f>
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="19">
-        <v>37</v>
-      </c>
-      <c r="C9" s="20">
-        <v>29</v>
-      </c>
-      <c r="D9" s="21">
-        <v>27</v>
-      </c>
-      <c r="E9" s="21">
-        <v>35</v>
-      </c>
-      <c r="F9" s="21">
-        <v>22</v>
-      </c>
-      <c r="G9" s="21">
-        <v>16</v>
-      </c>
-      <c r="H9" s="21">
-        <v>29</v>
-      </c>
-      <c r="I9" s="23">
+      <c r="B11" s="19">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20">
+        <v>1</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26">
+        <v>3</v>
+      </c>
+      <c r="J11" s="26">
+        <v>2</v>
+      </c>
+      <c r="K11" s="22">
+        <v>1</v>
+      </c>
+      <c r="L11" s="22">
+        <v>1</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="28">
+        <f>SUM(B11:M11)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="N12" s="30">
+        <f>SUM(B12:M12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="32">
+        <v>10</v>
+      </c>
+      <c r="C16" s="33">
+        <v>10</v>
+      </c>
+      <c r="D16" s="33">
         <v>20</v>
       </c>
-      <c r="J9" s="23">
-        <v>28</v>
-      </c>
-      <c r="K9" s="22">
-        <v>23</v>
-      </c>
-      <c r="L9" s="22">
-        <v>14</v>
-      </c>
-      <c r="M9" s="22">
-        <v>17</v>
-      </c>
-      <c r="N9" s="17">
-        <f>SUM(B9:M9)</f>
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.6">
-      <c r="A10" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="19">
-        <v>14</v>
-      </c>
-      <c r="C10" s="20">
-        <v>16</v>
-      </c>
-      <c r="D10" s="21">
-        <v>15</v>
-      </c>
-      <c r="E10" s="21">
-        <v>15</v>
-      </c>
-      <c r="F10" s="21">
-        <v>11</v>
-      </c>
-      <c r="G10" s="21">
+    </row>
+    <row r="17" spans="1:4" ht="62.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="35">
+        <v>25</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="37">
         <v>10</v>
       </c>
-      <c r="H10" s="21">
-        <v>11</v>
-      </c>
-      <c r="I10" s="23">
-        <v>12</v>
-      </c>
-      <c r="J10" s="23">
-        <v>14</v>
-      </c>
-      <c r="K10" s="22">
-        <v>4</v>
-      </c>
-      <c r="L10" s="22">
-        <v>8</v>
-      </c>
-      <c r="M10" s="22">
-        <v>11</v>
-      </c>
-      <c r="N10" s="17">
-        <f>SUM(B10:M10)</f>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.6">
-      <c r="A11" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="19">
-        <f>SUM(B7:B10)</f>
-        <v>124</v>
-      </c>
-      <c r="C11" s="19">
-        <f t="shared" ref="C11:M11" si="0">SUM(C7:C10)</f>
-        <v>121</v>
-      </c>
-      <c r="D11" s="19">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="E11" s="19">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="F11" s="19">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="G11" s="19">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="H11" s="19">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="I11" s="19">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="J11" s="19">
-        <f t="shared" si="0"/>
-        <v>137</v>
-      </c>
-      <c r="K11" s="19">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-      <c r="L11" s="19">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="M11" s="19">
-        <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-      <c r="N11" s="25">
-        <f>SUM(N7:N10)</f>
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="41.4">
-      <c r="A13" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="19">
-        <v>1</v>
-      </c>
-      <c r="C13" s="20">
-        <v>1</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26">
-        <v>3</v>
-      </c>
-      <c r="J13" s="26">
-        <v>2</v>
-      </c>
-      <c r="K13" s="22">
-        <v>1</v>
-      </c>
-      <c r="L13" s="22">
-        <v>1</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="N13" s="28">
-        <f>SUM(B13:M13)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="41.4">
-      <c r="A14" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="20">
-        <v>1</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="N14" s="30">
-        <f>SUM(B14:M14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="17.399999999999999">
-      <c r="A16" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="46.8">
-      <c r="A18" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="32">
-        <v>10</v>
-      </c>
-      <c r="C18" s="33">
-        <v>10</v>
-      </c>
-      <c r="D18" s="33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="62.4">
-      <c r="A19" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="35">
-        <v>25</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="46.8">
-      <c r="A20" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="37">
-        <v>10</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38">
+      <c r="C18" s="38"/>
+      <c r="D18" s="38">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3150,11 +3186,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76527AF-2381-4A84-92A9-FC93FB5C94DB}">
   <dimension ref="A1:O170"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10" style="59"/>
     <col min="3" max="3" width="11.5" style="59" customWidth="1"/>
@@ -3176,54 +3212,54 @@
     <col min="48" max="16384" width="10" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="105.6">
+    <row r="1" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="G1" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="H1" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="I1" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="N1" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="O1" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="O1" s="42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="46.8">
+    </row>
+    <row r="2" spans="1:15" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A2" s="44">
         <v>1</v>
       </c>
@@ -3231,16 +3267,16 @@
         <v>116</v>
       </c>
       <c r="C2" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="47" t="s">
         <v>152</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>155</v>
       </c>
       <c r="G2" s="48">
         <v>672</v>
@@ -3273,7 +3309,7 @@
         <v>3198</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="62.4">
+    <row r="3" spans="1:15" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A3" s="44">
         <v>2</v>
       </c>
@@ -3284,46 +3320,45 @@
         <v>55</v>
       </c>
       <c r="D3" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>156</v>
-      </c>
       <c r="F3" s="51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G3" s="52">
-        <v>859</v>
+        <v>187</v>
       </c>
       <c r="H3" s="52">
-        <v>837</v>
+        <v>246</v>
       </c>
       <c r="I3" s="52">
-        <v>596</v>
+        <v>170</v>
       </c>
       <c r="J3" s="52">
-        <v>630</v>
+        <v>235</v>
       </c>
       <c r="K3" s="52">
-        <v>750</v>
+        <v>215</v>
       </c>
       <c r="L3" s="52">
-        <v>802</v>
+        <v>223</v>
       </c>
       <c r="M3" s="48">
-        <f t="shared" ref="M3:M4" si="0">G3+I3+K3</f>
-        <v>2205</v>
+        <v>572</v>
       </c>
       <c r="N3" s="48">
-        <f t="shared" ref="N3:N4" si="1">H3+J3+L3</f>
-        <v>2269</v>
+        <f t="shared" ref="N3" si="0">H3+J3+L3</f>
+        <v>704</v>
       </c>
       <c r="O3" s="48">
         <f>M3+N3</f>
-        <v>4474</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="62.4">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="62.4" x14ac:dyDescent="0.25">
       <c r="A4" s="44">
         <v>3</v>
       </c>
@@ -3334,48 +3369,46 @@
         <v>55</v>
       </c>
       <c r="D4" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="49" t="s">
-        <v>156</v>
-      </c>
       <c r="F4" s="51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G4" s="52">
-        <v>1886</v>
+        <v>355</v>
       </c>
       <c r="H4" s="52">
-        <v>1912</v>
+        <v>484</v>
       </c>
       <c r="I4" s="52">
-        <v>1436</v>
+        <v>414</v>
       </c>
       <c r="J4" s="52">
-        <v>1380</v>
+        <v>355</v>
       </c>
       <c r="K4" s="52">
-        <v>1658</v>
+        <v>373</v>
       </c>
       <c r="L4" s="52">
-        <v>1631</v>
+        <v>250</v>
       </c>
       <c r="M4" s="48">
-        <f t="shared" si="0"/>
-        <v>4980</v>
+        <v>1142</v>
       </c>
       <c r="N4" s="48">
-        <f t="shared" si="1"/>
-        <v>4923</v>
+        <v>1089</v>
       </c>
       <c r="O4" s="48">
         <f>M4+N4</f>
-        <v>9903</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="95.55" customHeight="1">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="95.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
@@ -3384,44 +3417,44 @@
       <c r="F5" s="69"/>
       <c r="G5" s="53">
         <f>SUM(G2:G4)</f>
-        <v>3417</v>
+        <v>1214</v>
       </c>
       <c r="H5" s="53">
-        <f t="shared" ref="H5:O5" si="2">SUM(H2:H4)</f>
-        <v>3340</v>
+        <f t="shared" ref="H5:O5" si="1">SUM(H2:H4)</f>
+        <v>1321</v>
       </c>
       <c r="I5" s="53">
-        <f t="shared" si="2"/>
-        <v>2458</v>
+        <f t="shared" si="1"/>
+        <v>1010</v>
       </c>
       <c r="J5" s="53">
-        <f t="shared" si="2"/>
-        <v>2405</v>
+        <f t="shared" si="1"/>
+        <v>985</v>
       </c>
       <c r="K5" s="53">
-        <f t="shared" si="2"/>
-        <v>2943</v>
+        <f t="shared" si="1"/>
+        <v>1123</v>
       </c>
       <c r="L5" s="53">
-        <f t="shared" si="2"/>
-        <v>3012</v>
+        <f t="shared" si="1"/>
+        <v>1052</v>
       </c>
       <c r="M5" s="53">
-        <f t="shared" si="2"/>
-        <v>8818</v>
+        <f t="shared" si="1"/>
+        <v>3347</v>
       </c>
       <c r="N5" s="53">
-        <f t="shared" si="2"/>
-        <v>8757</v>
+        <f t="shared" si="1"/>
+        <v>3358</v>
       </c>
       <c r="O5" s="53">
-        <f t="shared" si="2"/>
-        <v>17575</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="31.2" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>6705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
@@ -3437,10 +3470,10 @@
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
       <c r="O6" s="54">
-        <v>17575</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>6705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="55"/>
       <c r="B7" s="56"/>
       <c r="C7" s="57"/>
@@ -3457,7 +3490,7 @@
       <c r="N7" s="55"/>
       <c r="O7" s="58"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="55"/>
       <c r="B8" s="56"/>
       <c r="C8" s="57"/>
@@ -3474,7 +3507,7 @@
       <c r="N8" s="55"/>
       <c r="O8" s="58"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="55"/>
       <c r="B9" s="56"/>
       <c r="C9" s="57"/>
@@ -3491,7 +3524,7 @@
       <c r="N9" s="55"/>
       <c r="O9" s="58"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="55"/>
       <c r="B10" s="56"/>
       <c r="C10" s="57"/>
@@ -3508,7 +3541,7 @@
       <c r="N10" s="55"/>
       <c r="O10" s="58"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="55"/>
       <c r="B11" s="56"/>
       <c r="C11" s="57"/>
@@ -3525,7 +3558,7 @@
       <c r="N11" s="55"/>
       <c r="O11" s="58"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="55"/>
       <c r="B12" s="56"/>
       <c r="C12" s="57"/>
@@ -3542,7 +3575,7 @@
       <c r="N12" s="55"/>
       <c r="O12" s="58"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="55"/>
       <c r="B13" s="56"/>
       <c r="C13" s="57"/>
@@ -3559,7 +3592,7 @@
       <c r="N13" s="55"/>
       <c r="O13" s="58"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="55"/>
       <c r="B14" s="55"/>
       <c r="C14" s="57"/>
@@ -3576,7 +3609,7 @@
       <c r="N14" s="55"/>
       <c r="O14" s="58"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
       <c r="B15" s="55"/>
       <c r="C15" s="57"/>
@@ -3593,7 +3626,7 @@
       <c r="N15" s="55"/>
       <c r="O15" s="58"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="55"/>
       <c r="B16" s="55"/>
       <c r="C16" s="57"/>
@@ -3610,7 +3643,7 @@
       <c r="N16" s="55"/>
       <c r="O16" s="58"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="57"/>
@@ -3627,7 +3660,7 @@
       <c r="N17" s="55"/>
       <c r="O17" s="58"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="55"/>
       <c r="B18" s="55"/>
       <c r="C18" s="57"/>
@@ -3644,7 +3677,7 @@
       <c r="N18" s="55"/>
       <c r="O18" s="58"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="55"/>
       <c r="B19" s="55"/>
       <c r="C19" s="57"/>
@@ -3661,7 +3694,7 @@
       <c r="N19" s="55"/>
       <c r="O19" s="58"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="55"/>
       <c r="B20" s="55"/>
       <c r="C20" s="57"/>
@@ -3678,7 +3711,7 @@
       <c r="N20" s="55"/>
       <c r="O20" s="58"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="55"/>
       <c r="B21" s="55"/>
       <c r="C21" s="57"/>
@@ -3695,7 +3728,7 @@
       <c r="N21" s="55"/>
       <c r="O21" s="58"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="55"/>
       <c r="B22" s="55"/>
       <c r="C22" s="57"/>
@@ -3712,7 +3745,7 @@
       <c r="N22" s="55"/>
       <c r="O22" s="58"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
       <c r="B23" s="55"/>
       <c r="C23" s="57"/>
@@ -3729,7 +3762,7 @@
       <c r="N23" s="55"/>
       <c r="O23" s="58"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
       <c r="B24" s="55"/>
       <c r="C24" s="57"/>
@@ -3746,7 +3779,7 @@
       <c r="N24" s="55"/>
       <c r="O24" s="58"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="55"/>
       <c r="B25" s="55"/>
       <c r="C25" s="57"/>
@@ -3763,7 +3796,7 @@
       <c r="N25" s="55"/>
       <c r="O25" s="58"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="55"/>
       <c r="B26" s="55"/>
       <c r="C26" s="57"/>
@@ -3780,7 +3813,7 @@
       <c r="N26" s="55"/>
       <c r="O26" s="58"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="55"/>
       <c r="B27" s="55"/>
       <c r="C27" s="57"/>
@@ -3797,7 +3830,7 @@
       <c r="N27" s="55"/>
       <c r="O27" s="58"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="55"/>
       <c r="B28" s="55"/>
       <c r="C28" s="57"/>
@@ -3814,7 +3847,7 @@
       <c r="N28" s="55"/>
       <c r="O28" s="58"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="55"/>
       <c r="B29" s="55"/>
       <c r="C29" s="57"/>
@@ -3831,7 +3864,7 @@
       <c r="N29" s="55"/>
       <c r="O29" s="58"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="55"/>
       <c r="B30" s="55"/>
       <c r="C30" s="57"/>
@@ -3848,7 +3881,7 @@
       <c r="N30" s="55"/>
       <c r="O30" s="58"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
       <c r="B31" s="55"/>
       <c r="C31" s="57"/>
@@ -3865,7 +3898,7 @@
       <c r="N31" s="55"/>
       <c r="O31" s="58"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
       <c r="B32" s="55"/>
       <c r="C32" s="57"/>
@@ -3882,7 +3915,7 @@
       <c r="N32" s="55"/>
       <c r="O32" s="58"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
       <c r="B33" s="55"/>
       <c r="C33" s="57"/>
@@ -3899,7 +3932,7 @@
       <c r="N33" s="55"/>
       <c r="O33" s="58"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="55"/>
       <c r="B34" s="55"/>
       <c r="C34" s="57"/>
@@ -3916,7 +3949,7 @@
       <c r="N34" s="55"/>
       <c r="O34" s="58"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="55"/>
       <c r="B35" s="55"/>
       <c r="C35" s="57"/>
@@ -3933,7 +3966,7 @@
       <c r="N35" s="55"/>
       <c r="O35" s="58"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="55"/>
       <c r="B36" s="55"/>
       <c r="C36" s="57"/>
@@ -3950,7 +3983,7 @@
       <c r="N36" s="55"/>
       <c r="O36" s="58"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="55"/>
       <c r="B37" s="55"/>
       <c r="C37" s="57"/>
@@ -3967,7 +4000,7 @@
       <c r="N37" s="55"/>
       <c r="O37" s="58"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="55"/>
       <c r="B38" s="55"/>
       <c r="C38" s="57"/>
@@ -3984,7 +4017,7 @@
       <c r="N38" s="55"/>
       <c r="O38" s="58"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="55"/>
       <c r="B39" s="55"/>
       <c r="C39" s="57"/>
@@ -4001,7 +4034,7 @@
       <c r="N39" s="55"/>
       <c r="O39" s="58"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
       <c r="B40" s="55"/>
       <c r="C40" s="57"/>
@@ -4018,7 +4051,7 @@
       <c r="N40" s="55"/>
       <c r="O40" s="58"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
       <c r="B41" s="55"/>
       <c r="C41" s="57"/>
@@ -4035,7 +4068,7 @@
       <c r="N41" s="55"/>
       <c r="O41" s="58"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
       <c r="B42" s="55"/>
       <c r="C42" s="57"/>
@@ -4052,7 +4085,7 @@
       <c r="N42" s="55"/>
       <c r="O42" s="58"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="55"/>
       <c r="B43" s="55"/>
       <c r="C43" s="57"/>
@@ -4069,7 +4102,7 @@
       <c r="N43" s="55"/>
       <c r="O43" s="58"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="55"/>
       <c r="B44" s="55"/>
       <c r="C44" s="57"/>
@@ -4086,7 +4119,7 @@
       <c r="N44" s="55"/>
       <c r="O44" s="58"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="55"/>
       <c r="B45" s="55"/>
       <c r="C45" s="57"/>
@@ -4103,7 +4136,7 @@
       <c r="N45" s="55"/>
       <c r="O45" s="58"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="55"/>
       <c r="B46" s="55"/>
       <c r="C46" s="57"/>
@@ -4120,7 +4153,7 @@
       <c r="N46" s="55"/>
       <c r="O46" s="58"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="55"/>
       <c r="B47" s="55"/>
       <c r="C47" s="57"/>
@@ -4137,7 +4170,7 @@
       <c r="N47" s="55"/>
       <c r="O47" s="58"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="55"/>
       <c r="B48" s="55"/>
       <c r="C48" s="57"/>
@@ -4154,7 +4187,7 @@
       <c r="N48" s="55"/>
       <c r="O48" s="58"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="55"/>
       <c r="B49" s="55"/>
       <c r="C49" s="57"/>
@@ -4171,7 +4204,7 @@
       <c r="N49" s="55"/>
       <c r="O49" s="58"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="55"/>
       <c r="B50" s="55"/>
       <c r="C50" s="57"/>
@@ -4188,7 +4221,7 @@
       <c r="N50" s="55"/>
       <c r="O50" s="58"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
       <c r="B51" s="55"/>
       <c r="C51" s="57"/>
@@ -4205,7 +4238,7 @@
       <c r="N51" s="55"/>
       <c r="O51" s="58"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
       <c r="B52" s="55"/>
       <c r="C52" s="57"/>
@@ -4222,7 +4255,7 @@
       <c r="N52" s="55"/>
       <c r="O52" s="58"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="55"/>
       <c r="B53" s="55"/>
       <c r="C53" s="57"/>
@@ -4239,7 +4272,7 @@
       <c r="N53" s="55"/>
       <c r="O53" s="58"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="55"/>
       <c r="B54" s="55"/>
       <c r="C54" s="57"/>
@@ -4256,7 +4289,7 @@
       <c r="N54" s="55"/>
       <c r="O54" s="58"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="55"/>
       <c r="B55" s="55"/>
       <c r="C55" s="57"/>
@@ -4273,7 +4306,7 @@
       <c r="N55" s="55"/>
       <c r="O55" s="58"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="55"/>
       <c r="B56" s="55"/>
       <c r="C56" s="57"/>
@@ -4290,7 +4323,7 @@
       <c r="N56" s="55"/>
       <c r="O56" s="58"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="55"/>
       <c r="B57" s="55"/>
       <c r="C57" s="57"/>
@@ -4307,7 +4340,7 @@
       <c r="N57" s="55"/>
       <c r="O57" s="58"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="55"/>
       <c r="B58" s="55"/>
       <c r="C58" s="57"/>
@@ -4324,7 +4357,7 @@
       <c r="N58" s="55"/>
       <c r="O58" s="58"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="55"/>
       <c r="B59" s="55"/>
       <c r="C59" s="57"/>
@@ -4341,7 +4374,7 @@
       <c r="N59" s="55"/>
       <c r="O59" s="58"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="55"/>
       <c r="B60" s="55"/>
       <c r="C60" s="57"/>
@@ -4358,7 +4391,7 @@
       <c r="N60" s="55"/>
       <c r="O60" s="58"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
       <c r="B61" s="55"/>
       <c r="C61" s="57"/>
@@ -4375,7 +4408,7 @@
       <c r="N61" s="55"/>
       <c r="O61" s="58"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="55"/>
       <c r="B62" s="55"/>
       <c r="C62" s="57"/>
@@ -4392,7 +4425,7 @@
       <c r="N62" s="55"/>
       <c r="O62" s="58"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="55"/>
       <c r="B63" s="55"/>
       <c r="C63" s="57"/>
@@ -4409,7 +4442,7 @@
       <c r="N63" s="55"/>
       <c r="O63" s="58"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="55"/>
       <c r="B64" s="55"/>
       <c r="C64" s="57"/>
@@ -4426,7 +4459,7 @@
       <c r="N64" s="55"/>
       <c r="O64" s="58"/>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="55"/>
       <c r="B65" s="55"/>
       <c r="C65" s="57"/>
@@ -4443,7 +4476,7 @@
       <c r="N65" s="55"/>
       <c r="O65" s="58"/>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="55"/>
       <c r="B66" s="55"/>
       <c r="C66" s="57"/>
@@ -4460,7 +4493,7 @@
       <c r="N66" s="55"/>
       <c r="O66" s="58"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="55"/>
       <c r="B67" s="55"/>
       <c r="C67" s="57"/>
@@ -4477,7 +4510,7 @@
       <c r="N67" s="55"/>
       <c r="O67" s="58"/>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="55"/>
       <c r="B68" s="55"/>
       <c r="C68" s="57"/>
@@ -4494,7 +4527,7 @@
       <c r="N68" s="55"/>
       <c r="O68" s="58"/>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="55"/>
       <c r="B69" s="55"/>
       <c r="C69" s="57"/>
@@ -4511,7 +4544,7 @@
       <c r="N69" s="55"/>
       <c r="O69" s="58"/>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="55"/>
       <c r="B70" s="55"/>
       <c r="C70" s="57"/>
@@ -4528,7 +4561,7 @@
       <c r="N70" s="55"/>
       <c r="O70" s="58"/>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="55"/>
       <c r="B71" s="55"/>
       <c r="C71" s="57"/>
@@ -4545,7 +4578,7 @@
       <c r="N71" s="55"/>
       <c r="O71" s="58"/>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="55"/>
       <c r="B72" s="55"/>
       <c r="C72" s="57"/>
@@ -4562,7 +4595,7 @@
       <c r="N72" s="55"/>
       <c r="O72" s="58"/>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="55"/>
       <c r="B73" s="55"/>
       <c r="C73" s="57"/>
@@ -4579,7 +4612,7 @@
       <c r="N73" s="55"/>
       <c r="O73" s="58"/>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="55"/>
       <c r="B74" s="55"/>
       <c r="C74" s="57"/>
@@ -4596,7 +4629,7 @@
       <c r="N74" s="55"/>
       <c r="O74" s="58"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="57"/>
@@ -4613,7 +4646,7 @@
       <c r="N75" s="55"/>
       <c r="O75" s="58"/>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="57"/>
@@ -4630,7 +4663,7 @@
       <c r="N76" s="55"/>
       <c r="O76" s="58"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="57"/>
@@ -4647,7 +4680,7 @@
       <c r="N77" s="55"/>
       <c r="O77" s="58"/>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="57"/>
@@ -4664,7 +4697,7 @@
       <c r="N78" s="55"/>
       <c r="O78" s="58"/>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="55"/>
       <c r="B79" s="55"/>
       <c r="C79" s="57"/>
@@ -4681,7 +4714,7 @@
       <c r="N79" s="55"/>
       <c r="O79" s="58"/>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="55"/>
       <c r="B80" s="55"/>
       <c r="C80" s="57"/>
@@ -4698,7 +4731,7 @@
       <c r="N80" s="55"/>
       <c r="O80" s="58"/>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="55"/>
       <c r="B81" s="55"/>
       <c r="C81" s="57"/>
@@ -4715,7 +4748,7 @@
       <c r="N81" s="55"/>
       <c r="O81" s="58"/>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="55"/>
       <c r="B82" s="55"/>
       <c r="C82" s="57"/>
@@ -4732,7 +4765,7 @@
       <c r="N82" s="55"/>
       <c r="O82" s="58"/>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="55"/>
       <c r="B83" s="55"/>
       <c r="C83" s="57"/>
@@ -4749,7 +4782,7 @@
       <c r="N83" s="55"/>
       <c r="O83" s="58"/>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="55"/>
       <c r="B84" s="55"/>
       <c r="C84" s="57"/>
@@ -4766,7 +4799,7 @@
       <c r="N84" s="55"/>
       <c r="O84" s="58"/>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="55"/>
       <c r="B85" s="55"/>
       <c r="C85" s="57"/>
@@ -4783,7 +4816,7 @@
       <c r="N85" s="55"/>
       <c r="O85" s="58"/>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="55"/>
       <c r="B86" s="55"/>
       <c r="C86" s="57"/>
@@ -4800,7 +4833,7 @@
       <c r="N86" s="55"/>
       <c r="O86" s="58"/>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="55"/>
       <c r="B87" s="55"/>
       <c r="C87" s="57"/>
@@ -4817,7 +4850,7 @@
       <c r="N87" s="55"/>
       <c r="O87" s="58"/>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="55"/>
       <c r="B88" s="55"/>
       <c r="C88" s="57"/>
@@ -4834,7 +4867,7 @@
       <c r="N88" s="55"/>
       <c r="O88" s="58"/>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="55"/>
       <c r="B89" s="55"/>
       <c r="C89" s="57"/>
@@ -4851,7 +4884,7 @@
       <c r="N89" s="55"/>
       <c r="O89" s="58"/>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="55"/>
       <c r="B90" s="55"/>
       <c r="C90" s="57"/>
@@ -4868,7 +4901,7 @@
       <c r="N90" s="55"/>
       <c r="O90" s="58"/>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="55"/>
       <c r="B91" s="55"/>
       <c r="C91" s="57"/>
@@ -4885,7 +4918,7 @@
       <c r="N91" s="55"/>
       <c r="O91" s="58"/>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="55"/>
       <c r="B92" s="55"/>
       <c r="C92" s="57"/>
@@ -4902,7 +4935,7 @@
       <c r="N92" s="55"/>
       <c r="O92" s="58"/>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="55"/>
       <c r="B93" s="55"/>
       <c r="C93" s="57"/>
@@ -4919,7 +4952,7 @@
       <c r="N93" s="55"/>
       <c r="O93" s="58"/>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="55"/>
       <c r="B94" s="55"/>
       <c r="C94" s="57"/>
@@ -4936,7 +4969,7 @@
       <c r="N94" s="55"/>
       <c r="O94" s="58"/>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="55"/>
       <c r="B95" s="55"/>
       <c r="C95" s="57"/>
@@ -4953,7 +4986,7 @@
       <c r="N95" s="55"/>
       <c r="O95" s="58"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="55"/>
       <c r="B96" s="55"/>
       <c r="C96" s="57"/>
@@ -4970,7 +5003,7 @@
       <c r="N96" s="55"/>
       <c r="O96" s="58"/>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="55"/>
       <c r="B97" s="55"/>
       <c r="C97" s="57"/>
@@ -4987,7 +5020,7 @@
       <c r="N97" s="55"/>
       <c r="O97" s="58"/>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="55"/>
       <c r="B98" s="55"/>
       <c r="C98" s="57"/>
@@ -5004,7 +5037,7 @@
       <c r="N98" s="55"/>
       <c r="O98" s="58"/>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="55"/>
       <c r="B99" s="55"/>
       <c r="C99" s="57"/>
@@ -5021,7 +5054,7 @@
       <c r="N99" s="55"/>
       <c r="O99" s="58"/>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="55"/>
       <c r="B100" s="55"/>
       <c r="C100" s="57"/>
@@ -5038,7 +5071,7 @@
       <c r="N100" s="55"/>
       <c r="O100" s="58"/>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="55"/>
       <c r="B101" s="55"/>
       <c r="C101" s="57"/>
@@ -5055,7 +5088,7 @@
       <c r="N101" s="55"/>
       <c r="O101" s="58"/>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="55"/>
       <c r="B102" s="55"/>
       <c r="C102" s="57"/>
@@ -5072,7 +5105,7 @@
       <c r="N102" s="55"/>
       <c r="O102" s="58"/>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="55"/>
       <c r="B103" s="55"/>
       <c r="C103" s="57"/>
@@ -5089,7 +5122,7 @@
       <c r="N103" s="55"/>
       <c r="O103" s="58"/>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="55"/>
       <c r="B104" s="55"/>
       <c r="C104" s="57"/>
@@ -5106,7 +5139,7 @@
       <c r="N104" s="55"/>
       <c r="O104" s="58"/>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="55"/>
       <c r="B105" s="55"/>
       <c r="C105" s="57"/>
@@ -5123,7 +5156,7 @@
       <c r="N105" s="55"/>
       <c r="O105" s="58"/>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="55"/>
       <c r="B106" s="55"/>
       <c r="C106" s="57"/>
@@ -5140,7 +5173,7 @@
       <c r="N106" s="55"/>
       <c r="O106" s="58"/>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="55"/>
       <c r="B107" s="55"/>
       <c r="C107" s="57"/>
@@ -5157,7 +5190,7 @@
       <c r="N107" s="55"/>
       <c r="O107" s="58"/>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="55"/>
       <c r="B108" s="55"/>
       <c r="C108" s="57"/>
@@ -5174,7 +5207,7 @@
       <c r="N108" s="55"/>
       <c r="O108" s="58"/>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="55"/>
       <c r="B109" s="55"/>
       <c r="C109" s="57"/>
@@ -5191,7 +5224,7 @@
       <c r="N109" s="55"/>
       <c r="O109" s="58"/>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="55"/>
       <c r="B110" s="55"/>
       <c r="C110" s="57"/>
@@ -5208,7 +5241,7 @@
       <c r="N110" s="55"/>
       <c r="O110" s="58"/>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="55"/>
       <c r="B111" s="55"/>
       <c r="C111" s="57"/>
@@ -5225,7 +5258,7 @@
       <c r="N111" s="55"/>
       <c r="O111" s="58"/>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="55"/>
       <c r="B112" s="55"/>
       <c r="C112" s="57"/>
@@ -5242,7 +5275,7 @@
       <c r="N112" s="55"/>
       <c r="O112" s="58"/>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="55"/>
       <c r="B113" s="55"/>
       <c r="C113" s="57"/>
@@ -5259,7 +5292,7 @@
       <c r="N113" s="55"/>
       <c r="O113" s="58"/>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="55"/>
       <c r="B114" s="55"/>
       <c r="C114" s="57"/>
@@ -5276,7 +5309,7 @@
       <c r="N114" s="55"/>
       <c r="O114" s="58"/>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="55"/>
       <c r="B115" s="55"/>
       <c r="C115" s="57"/>
@@ -5293,7 +5326,7 @@
       <c r="N115" s="55"/>
       <c r="O115" s="58"/>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="55"/>
       <c r="B116" s="55"/>
       <c r="C116" s="57"/>
@@ -5310,7 +5343,7 @@
       <c r="N116" s="55"/>
       <c r="O116" s="58"/>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="55"/>
       <c r="B117" s="55"/>
       <c r="C117" s="57"/>
@@ -5327,7 +5360,7 @@
       <c r="N117" s="55"/>
       <c r="O117" s="58"/>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="55"/>
       <c r="B118" s="55"/>
       <c r="C118" s="57"/>
@@ -5344,7 +5377,7 @@
       <c r="N118" s="55"/>
       <c r="O118" s="58"/>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="55"/>
       <c r="B119" s="55"/>
       <c r="C119" s="57"/>
@@ -5361,7 +5394,7 @@
       <c r="N119" s="55"/>
       <c r="O119" s="58"/>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="55"/>
       <c r="B120" s="55"/>
       <c r="C120" s="57"/>
@@ -5378,7 +5411,7 @@
       <c r="N120" s="55"/>
       <c r="O120" s="58"/>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="55"/>
       <c r="B121" s="55"/>
       <c r="C121" s="57"/>
@@ -5395,7 +5428,7 @@
       <c r="N121" s="55"/>
       <c r="O121" s="58"/>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="55"/>
       <c r="B122" s="55"/>
       <c r="C122" s="57"/>
@@ -5412,7 +5445,7 @@
       <c r="N122" s="55"/>
       <c r="O122" s="58"/>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="55"/>
       <c r="B123" s="55"/>
       <c r="C123" s="57"/>
@@ -5429,7 +5462,7 @@
       <c r="N123" s="55"/>
       <c r="O123" s="58"/>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="55"/>
       <c r="B124" s="55"/>
       <c r="C124" s="57"/>
@@ -5446,7 +5479,7 @@
       <c r="N124" s="55"/>
       <c r="O124" s="58"/>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="55"/>
       <c r="B125" s="55"/>
       <c r="C125" s="57"/>
@@ -5463,7 +5496,7 @@
       <c r="N125" s="55"/>
       <c r="O125" s="58"/>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="55"/>
       <c r="B126" s="55"/>
       <c r="C126" s="57"/>
@@ -5480,7 +5513,7 @@
       <c r="N126" s="55"/>
       <c r="O126" s="58"/>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="55"/>
       <c r="B127" s="55"/>
       <c r="C127" s="57"/>
@@ -5497,7 +5530,7 @@
       <c r="N127" s="55"/>
       <c r="O127" s="58"/>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="55"/>
       <c r="B128" s="55"/>
       <c r="C128" s="57"/>
@@ -5514,7 +5547,7 @@
       <c r="N128" s="55"/>
       <c r="O128" s="58"/>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="55"/>
       <c r="B129" s="55"/>
       <c r="C129" s="57"/>
@@ -5531,7 +5564,7 @@
       <c r="N129" s="55"/>
       <c r="O129" s="58"/>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="55"/>
       <c r="B130" s="55"/>
       <c r="C130" s="57"/>
@@ -5548,7 +5581,7 @@
       <c r="N130" s="55"/>
       <c r="O130" s="58"/>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="55"/>
       <c r="B131" s="55"/>
       <c r="C131" s="57"/>
@@ -5565,7 +5598,7 @@
       <c r="N131" s="55"/>
       <c r="O131" s="58"/>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="55"/>
       <c r="B132" s="55"/>
       <c r="C132" s="57"/>
@@ -5582,7 +5615,7 @@
       <c r="N132" s="55"/>
       <c r="O132" s="58"/>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="55"/>
       <c r="B133" s="55"/>
       <c r="C133" s="57"/>
@@ -5599,7 +5632,7 @@
       <c r="N133" s="55"/>
       <c r="O133" s="58"/>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="55"/>
       <c r="B134" s="55"/>
       <c r="C134" s="57"/>
@@ -5616,7 +5649,7 @@
       <c r="N134" s="55"/>
       <c r="O134" s="58"/>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="55"/>
       <c r="B135" s="55"/>
       <c r="C135" s="57"/>
@@ -5633,7 +5666,7 @@
       <c r="N135" s="55"/>
       <c r="O135" s="58"/>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="55"/>
       <c r="B136" s="55"/>
       <c r="C136" s="57"/>
@@ -5650,7 +5683,7 @@
       <c r="N136" s="55"/>
       <c r="O136" s="58"/>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="55"/>
       <c r="B137" s="55"/>
       <c r="C137" s="57"/>
@@ -5667,7 +5700,7 @@
       <c r="N137" s="55"/>
       <c r="O137" s="58"/>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="55"/>
       <c r="B138" s="55"/>
       <c r="C138" s="57"/>
@@ -5684,7 +5717,7 @@
       <c r="N138" s="55"/>
       <c r="O138" s="58"/>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="55"/>
       <c r="B139" s="55"/>
       <c r="C139" s="57"/>
@@ -5701,7 +5734,7 @@
       <c r="N139" s="55"/>
       <c r="O139" s="58"/>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="55"/>
       <c r="B140" s="55"/>
       <c r="C140" s="57"/>
@@ -5718,7 +5751,7 @@
       <c r="N140" s="55"/>
       <c r="O140" s="58"/>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="55"/>
       <c r="B141" s="55"/>
       <c r="C141" s="57"/>
@@ -5735,7 +5768,7 @@
       <c r="N141" s="55"/>
       <c r="O141" s="58"/>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="55"/>
       <c r="B142" s="55"/>
       <c r="C142" s="57"/>
@@ -5752,7 +5785,7 @@
       <c r="N142" s="55"/>
       <c r="O142" s="58"/>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="55"/>
       <c r="B143" s="55"/>
       <c r="C143" s="57"/>
@@ -5769,7 +5802,7 @@
       <c r="N143" s="55"/>
       <c r="O143" s="58"/>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="55"/>
       <c r="B144" s="55"/>
       <c r="C144" s="57"/>
@@ -5786,7 +5819,7 @@
       <c r="N144" s="55"/>
       <c r="O144" s="58"/>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="55"/>
       <c r="B145" s="55"/>
       <c r="C145" s="57"/>
@@ -5803,7 +5836,7 @@
       <c r="N145" s="55"/>
       <c r="O145" s="58"/>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="55"/>
       <c r="B146" s="55"/>
       <c r="C146" s="57"/>
@@ -5820,7 +5853,7 @@
       <c r="N146" s="55"/>
       <c r="O146" s="58"/>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="55"/>
       <c r="B147" s="55"/>
       <c r="C147" s="57"/>
@@ -5837,7 +5870,7 @@
       <c r="N147" s="55"/>
       <c r="O147" s="58"/>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="55"/>
       <c r="B148" s="55"/>
       <c r="C148" s="57"/>
@@ -5854,7 +5887,7 @@
       <c r="N148" s="55"/>
       <c r="O148" s="58"/>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="55"/>
       <c r="B149" s="55"/>
       <c r="C149" s="57"/>
@@ -5871,7 +5904,7 @@
       <c r="N149" s="55"/>
       <c r="O149" s="58"/>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="55"/>
       <c r="B150" s="55"/>
       <c r="C150" s="57"/>
@@ -5888,7 +5921,7 @@
       <c r="N150" s="55"/>
       <c r="O150" s="58"/>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="55"/>
       <c r="B151" s="55"/>
       <c r="C151" s="57"/>
@@ -5905,7 +5938,7 @@
       <c r="N151" s="55"/>
       <c r="O151" s="58"/>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="55"/>
       <c r="B152" s="55"/>
       <c r="C152" s="57"/>
@@ -5922,7 +5955,7 @@
       <c r="N152" s="55"/>
       <c r="O152" s="58"/>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="55"/>
       <c r="B153" s="55"/>
       <c r="C153" s="57"/>
@@ -5939,7 +5972,7 @@
       <c r="N153" s="55"/>
       <c r="O153" s="58"/>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="55"/>
       <c r="B154" s="55"/>
       <c r="C154" s="57"/>
@@ -5956,7 +5989,7 @@
       <c r="N154" s="55"/>
       <c r="O154" s="58"/>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="55"/>
       <c r="B155" s="55"/>
       <c r="C155" s="57"/>
@@ -5973,7 +6006,7 @@
       <c r="N155" s="55"/>
       <c r="O155" s="58"/>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="55"/>
       <c r="B156" s="55"/>
       <c r="C156" s="57"/>
@@ -5990,7 +6023,7 @@
       <c r="N156" s="55"/>
       <c r="O156" s="58"/>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" s="55"/>
       <c r="B157" s="55"/>
       <c r="C157" s="57"/>
@@ -6007,7 +6040,7 @@
       <c r="N157" s="55"/>
       <c r="O157" s="58"/>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="55"/>
       <c r="B158" s="55"/>
       <c r="C158" s="57"/>
@@ -6024,7 +6057,7 @@
       <c r="N158" s="55"/>
       <c r="O158" s="58"/>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="55"/>
       <c r="B159" s="55"/>
       <c r="C159" s="57"/>
@@ -6041,7 +6074,7 @@
       <c r="N159" s="55"/>
       <c r="O159" s="58"/>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="55"/>
       <c r="B160" s="55"/>
       <c r="C160" s="57"/>
@@ -6058,7 +6091,7 @@
       <c r="N160" s="55"/>
       <c r="O160" s="58"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="55"/>
       <c r="B161" s="55"/>
       <c r="C161" s="57"/>
@@ -6075,7 +6108,7 @@
       <c r="N161" s="55"/>
       <c r="O161" s="58"/>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="55"/>
       <c r="B162" s="55"/>
       <c r="C162" s="57"/>
@@ -6092,7 +6125,7 @@
       <c r="N162" s="55"/>
       <c r="O162" s="58"/>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="55"/>
       <c r="B163" s="55"/>
       <c r="C163" s="57"/>
@@ -6109,7 +6142,7 @@
       <c r="N163" s="55"/>
       <c r="O163" s="58"/>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="55"/>
       <c r="B164" s="55"/>
       <c r="C164" s="57"/>
@@ -6126,7 +6159,7 @@
       <c r="N164" s="55"/>
       <c r="O164" s="58"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="55"/>
       <c r="B165" s="55"/>
       <c r="C165" s="57"/>
@@ -6143,7 +6176,7 @@
       <c r="N165" s="55"/>
       <c r="O165" s="58"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="55"/>
       <c r="B166" s="55"/>
       <c r="C166" s="57"/>
@@ -6160,7 +6193,7 @@
       <c r="N166" s="55"/>
       <c r="O166" s="58"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="55"/>
       <c r="B167" s="55"/>
       <c r="C167" s="57"/>
@@ -6177,7 +6210,7 @@
       <c r="N167" s="55"/>
       <c r="O167" s="58"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="55"/>
       <c r="B168" s="55"/>
       <c r="C168" s="57"/>
@@ -6194,7 +6227,7 @@
       <c r="N168" s="55"/>
       <c r="O168" s="58"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="55"/>
       <c r="B169" s="55"/>
       <c r="C169" s="57"/>
@@ -6211,7 +6244,7 @@
       <c r="N169" s="55"/>
       <c r="O169" s="58"/>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="55"/>
       <c r="B170" s="55"/>
       <c r="C170" s="57"/>
@@ -6246,7 +6279,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.09765625" style="62" customWidth="1"/>
     <col min="2" max="3" width="14.5" style="62" customWidth="1"/>
@@ -6255,24 +6288,24 @@
     <col min="6" max="16384" width="8.796875" style="62"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="16.8" customHeight="1">
+    <row r="2" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B2" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.8" customHeight="1">
+    </row>
+    <row r="3" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>108</v>
       </c>
@@ -6289,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" customHeight="1">
+    <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>109</v>
       </c>
@@ -6306,9 +6339,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" customHeight="1">
+    <row r="5" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B5" s="62">
         <v>25</v>
@@ -6323,9 +6356,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.8" customHeight="1">
+    <row r="6" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B6" s="62">
         <v>24</v>
@@ -6340,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.8" customHeight="1">
+    <row r="7" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>112</v>
       </c>
@@ -6357,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.8" customHeight="1">
+    <row r="8" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>113</v>
       </c>
@@ -6374,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.8" customHeight="1">
+    <row r="9" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>114</v>
       </c>
@@ -6391,7 +6424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.8" customHeight="1">
+    <row r="10" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>115</v>
       </c>
@@ -6408,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.8" customHeight="1">
+    <row r="11" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>116</v>
       </c>
@@ -6425,7 +6458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.8" customHeight="1">
+    <row r="12" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>117</v>
       </c>
@@ -6442,7 +6475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.8" customHeight="1">
+    <row r="13" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>118</v>
       </c>
@@ -6459,7 +6492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.8" customHeight="1">
+    <row r="14" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>119</v>
       </c>
@@ -6476,9 +6509,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" s="62">
         <f>SUBTOTAL(109,الجدول13[الفلج])</f>
@@ -6503,4 +6536,218 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9C4E95-A3C1-4708-8B7A-ED46EC532F4F}">
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="8.796875" style="62"/>
+    <col min="6" max="6" width="12.3984375" style="62" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" style="62" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="73">
+        <v>1</v>
+      </c>
+      <c r="E3" s="73">
+        <v>20</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="73" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="74"/>
+      <c r="C4" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="73">
+        <v>4</v>
+      </c>
+      <c r="E4" s="73">
+        <v>69</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="76">
+        <v>1</v>
+      </c>
+      <c r="E5" s="76">
+        <v>20</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="77"/>
+      <c r="C6" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="76">
+        <v>4</v>
+      </c>
+      <c r="E6" s="76">
+        <v>72</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="73">
+        <v>1</v>
+      </c>
+      <c r="E7" s="73">
+        <v>20</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="74"/>
+      <c r="C8" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="73">
+        <v>4</v>
+      </c>
+      <c r="E8" s="73">
+        <v>61</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="73" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="76">
+        <v>1</v>
+      </c>
+      <c r="E9" s="76">
+        <v>20</v>
+      </c>
+      <c r="F9" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="77"/>
+      <c r="C10" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="76">
+        <v>5</v>
+      </c>
+      <c r="E10" s="76">
+        <v>80</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79">
+        <f>SUM(D3:D10)</f>
+        <v>21</v>
+      </c>
+      <c r="E11" s="79">
+        <f>SUM(E3:E10)</f>
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>